<commit_message>
update image format and size
</commit_message>
<xml_diff>
--- a/SEO-audit.xlsx
+++ b/SEO-audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OPENCLASSROOMS\PROJECT 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A6B99D-4708-4A2C-AEE6-9E7BA6268574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F91C80A-CD7C-457E-9E91-F5837664E21E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
   <si>
     <t>Category</t>
   </si>
@@ -142,10 +142,6 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>Adjust image size to fit the cointainer</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>https://web.dev/uses-responsive-images/?utm_source=lighthouse&amp;utm_medium=devtools</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
@@ -163,10 +159,6 @@
   </si>
   <si>
     <t>Using WebP, webmasters and web developers can create smaller, richer images that make the web faster.</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Convert all images to WebP format</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
@@ -264,6 +256,39 @@
   </si>
   <si>
     <t>The form at the contact area of page2 does not apply the css correctly</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rename footer area Directories' names</t>
+  </si>
+  <si>
+    <t>Change the link of the websites at footer area</t>
+  </si>
+  <si>
+    <t>Change the unuseful website at footer area</t>
+  </si>
+  <si>
+    <t>Reduce repeat keywords at head area</t>
+  </si>
+  <si>
+    <t>Hide the keywords shown on the title area</t>
+  </si>
+  <si>
+    <t>adjust the img for "I create website...." and "Mike's an..." for tablet and mobile version</t>
+  </si>
+  <si>
+    <t>adjust the social media icons align style at footer area of mobile version.</t>
+  </si>
+  <si>
+    <t>remove alt spam and useless words at img link</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adjust image "atlanta made sign orange" and "atlanta web designer mike" sizes to 1080P to fit the cointainer</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Convert some images to WebP format</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -331,7 +356,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -342,6 +367,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF7030A0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -365,7 +396,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -401,6 +432,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -619,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.27734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -694,7 +728,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>12</v>
@@ -714,7 +748,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>16</v>
@@ -734,7 +768,7 @@
         <v>18</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>20</v>
@@ -767,8 +801,8 @@
       <c r="A7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>32</v>
+      <c r="B7" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>28</v>
@@ -777,30 +811,30 @@
         <v>27</v>
       </c>
       <c r="E7" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>29</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="59.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="D8" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="45" x14ac:dyDescent="0.4">
@@ -808,19 +842,19 @@
         <v>26</v>
       </c>
       <c r="B9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>40</v>
-      </c>
       <c r="F9" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.4">
@@ -828,19 +862,19 @@
         <v>26</v>
       </c>
       <c r="B10" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="D10" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -848,109 +882,139 @@
         <v>26</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>47</v>
-      </c>
       <c r="E11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="53.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>54</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="73.150000000000006" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>56</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="10" t="s">
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:26" ht="58.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="10"/>
+    </row>
+    <row r="15" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="1:26" ht="86.65" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="10" t="s">
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="10"/>
-    </row>
-    <row r="15" spans="1:26" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="10" t="s">
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B17" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="E16" s="10"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.4">
       <c r="E17" s="10"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B18" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="E18" s="10"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B19" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="E19" s="10"/>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B20" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="E20" s="10"/>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" ht="39.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>63</v>
+      </c>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="E23" s="10"/>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="E24" s="10"/>
     </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="E25" s="10"/>
     </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="E26" s="10"/>
     </row>
-    <row r="27" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="E27" s="10"/>
     </row>
-    <row r="28" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E28" s="10"/>
     </row>
-    <row r="29" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E29" s="10"/>
     </row>
-    <row r="30" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E30" s="10"/>
     </row>
-    <row r="31" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E31" s="10"/>
     </row>
-    <row r="32" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E32" s="10"/>
     </row>
     <row r="33" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -962,7 +1026,9 @@
     <row r="35" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E35" s="10"/>
     </row>
-    <row r="36" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="36" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E36" s="10"/>
+    </row>
     <row r="37" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="38" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="39" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1927,6 +1993,7 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -1942,6 +2009,6 @@
     <hyperlink ref="F12" r:id="rId10" xr:uid="{AD3854B2-D1B6-442A-8257-485717595CD9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add tile and script defer attributes
</commit_message>
<xml_diff>
--- a/SEO-audit.xlsx
+++ b/SEO-audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OPENCLASSROOMS\PROJECT 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F91C80A-CD7C-457E-9E91-F5837664E21E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3689F056-9BE3-435D-AAEC-5690798FA4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -656,7 +656,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.27734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -861,7 +861,7 @@
       <c r="A10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="13" t="s">
         <v>40</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -901,7 +901,7 @@
       <c r="A12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="13" t="s">
         <v>54</v>
       </c>
       <c r="E12" s="10"/>

</xml_diff>

<commit_message>
adjust colors for contrast ratio add lang attribute add aria-label to social media link Hide the keywords shown on the header and footer area
</commit_message>
<xml_diff>
--- a/SEO-audit.xlsx
+++ b/SEO-audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OPENCLASSROOMS\PROJECT 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3689F056-9BE3-435D-AAEC-5690798FA4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACC4423-34BA-4045-ADFF-61E444F60013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -268,27 +268,29 @@
     <t>Change the unuseful website at footer area</t>
   </si>
   <si>
+    <t>adjust the img for "I create website...." and "Mike's an..." for tablet and mobile version</t>
+  </si>
+  <si>
+    <t>adjust the social media icons align style at footer area of mobile version.</t>
+  </si>
+  <si>
+    <t>remove alt spam and useless words at img link</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adjust image "atlanta made sign orange" and "atlanta web designer mike" sizes to 1080P to fit the cointainer</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Convert some images to WebP format</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
     <t>Reduce repeat keywords at head area</t>
-  </si>
-  <si>
-    <t>Hide the keywords shown on the title area</t>
-  </si>
-  <si>
-    <t>adjust the img for "I create website...." and "Mike's an..." for tablet and mobile version</t>
-  </si>
-  <si>
-    <t>adjust the social media icons align style at footer area of mobile version.</t>
-  </si>
-  <si>
-    <t>remove alt spam and useless words at img link</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Adjust image "atlanta made sign orange" and "atlanta web designer mike" sizes to 1080P to fit the cointainer</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Convert some images to WebP format</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hide the keywords shown on the header and footer area</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -371,7 +373,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF00FF99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -444,6 +446,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -655,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.27734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -721,7 +728,7 @@
       <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -741,7 +748,7 @@
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -761,7 +768,7 @@
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="13" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -811,7 +818,7 @@
         <v>27</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>29</v>
@@ -831,7 +838,7 @@
         <v>47</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>30</v>
@@ -958,20 +965,20 @@
       <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B19" s="8" t="s">
-        <v>61</v>
+      <c r="B19" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="E19" s="10"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B20" s="8" t="s">
-        <v>62</v>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.4">
+      <c r="B20" s="13" t="s">
+        <v>67</v>
       </c>
       <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:5" ht="39.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B21" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E21" s="10"/>
     </row>
@@ -980,13 +987,13 @@
         <v>8</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E22" s="10"/>
     </row>
     <row r="23" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B23" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E23" s="10"/>
     </row>

</xml_diff>

<commit_message>
fix page2 css import
</commit_message>
<xml_diff>
--- a/SEO-audit.xlsx
+++ b/SEO-audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OPENCLASSROOMS\PROJECT 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACC4423-34BA-4045-ADFF-61E444F60013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B2D699-0A54-44B3-B0A8-A49BD02B9135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
   <si>
     <t>Category</t>
   </si>
@@ -251,23 +251,9 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>Incorrect layout of the navigation area in page2</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>The form at the contact area of page2 does not apply the css correctly</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>Rename footer area Directories' names</t>
   </si>
   <si>
-    <t>Change the link of the websites at footer area</t>
-  </si>
-  <si>
-    <t>Change the unuseful website at footer area</t>
-  </si>
-  <si>
     <t>adjust the img for "I create website...." and "Mike's an..." for tablet and mobile version</t>
   </si>
   <si>
@@ -291,6 +277,10 @@
   </si>
   <si>
     <t>Hide the keywords shown on the header and footer area</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>page2 does not apply the css correctly</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -660,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.27734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -818,7 +808,7 @@
         <v>27</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>29</v>
@@ -838,7 +828,7 @@
         <v>47</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>30</v>
@@ -904,109 +894,109 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="53.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A12" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E12" s="10"/>
-      <c r="F12" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A13" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>55</v>
+      <c r="B13" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="E13" s="10"/>
     </row>
-    <row r="14" spans="1:26" ht="58.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" ht="30" x14ac:dyDescent="0.4">
       <c r="A14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>56</v>
+      <c r="B14" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="E14" s="10"/>
     </row>
-    <row r="15" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" ht="53.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>57</v>
+      <c r="B15" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="E15" s="10"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="F15" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="1:5" ht="39.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="10"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B17" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B18" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B19" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.4">
-      <c r="B20" s="13" t="s">
-        <v>67</v>
-      </c>
       <c r="E20" s="10"/>
     </row>
-    <row r="21" spans="1:5" ht="39.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="10" t="s">
-        <v>63</v>
-      </c>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>61</v>
-      </c>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="8" t="s">
-        <v>62</v>
-      </c>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="E23" s="10"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="E24" s="10"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E25" s="10"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E26" s="10"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E27" s="10"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1027,15 +1017,9 @@
     <row r="33" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E33" s="10"/>
     </row>
-    <row r="34" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="E34" s="10"/>
-    </row>
-    <row r="35" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="E35" s="10"/>
-    </row>
-    <row r="36" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="E36" s="10"/>
-    </row>
+    <row r="34" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="35" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="36" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="37" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="38" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="39" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1998,9 +1982,6 @@
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -2013,7 +1994,7 @@
     <hyperlink ref="F9" r:id="rId7" xr:uid="{66F7160D-E8A6-449A-A5A8-658623D5755F}"/>
     <hyperlink ref="F10" r:id="rId8" xr:uid="{90D560FD-8AB3-40D1-A390-4ABEF3D97AF8}"/>
     <hyperlink ref="F11" r:id="rId9" display="https://web.dev/unused-css-rules/?utm_source=lighthouse&amp;utm_medium=devtools" xr:uid="{7B2C1893-7DB7-49FC-B823-A385BB686396}"/>
-    <hyperlink ref="F12" r:id="rId10" xr:uid="{AD3854B2-D1B6-442A-8257-485717595CD9}"/>
+    <hyperlink ref="F15" r:id="rId10" xr:uid="{AD3854B2-D1B6-442A-8257-485717595CD9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId11"/>

</xml_diff>

<commit_message>
name the page regions
</commit_message>
<xml_diff>
--- a/SEO-audit.xlsx
+++ b/SEO-audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OPENCLASSROOMS\PROJECT 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B2D699-0A54-44B3-B0A8-A49BD02B9135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327497B4-DFCB-4D84-82F0-155D687821AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -652,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.27734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -778,7 +778,7 @@
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="10" t="s">

</xml_diff>

<commit_message>
add page2 headings add preload for fonts add alt for page2 logo fix the same problems on page2
</commit_message>
<xml_diff>
--- a/SEO-audit.xlsx
+++ b/SEO-audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OPENCLASSROOMS\PROJECT 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327497B4-DFCB-4D84-82F0-155D687821AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACD2225-061F-4491-9242-2CA758CE5D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="75">
   <si>
     <t>Category</t>
   </si>
@@ -282,6 +282,45 @@
   <si>
     <t>page2 does not apply the css correctly</t>
     <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://web.dev/bypass/?utm_source=lighthouse&amp;utm_medium=devtools</t>
+  </si>
+  <si>
+    <t>The page does not contain a heading, skip link, or landmark region (Page 2)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Providing a way to bypass repetitive content makes non-mouse navigation easier.</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Make sure each pages have a heading.</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>add heading tag to page2</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Image elements do not have [alt] attributes (Page 2)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Informative elements should aim for short, descriptive alternate text.</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Make sure each img have a [alt] attributes.</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>add [alt] attributes to logo img.</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://web.dev/image-alt/?utm_source=lighthouse&amp;utm_medium=devtools</t>
   </si>
 </sst>
 </file>
@@ -650,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.27734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -794,231 +833,269 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="85.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:26" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="9" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="59.65" customHeight="1" x14ac:dyDescent="0.4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="9" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="45" x14ac:dyDescent="0.4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="85.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>36</v>
+      <c r="B9" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="59.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="45" x14ac:dyDescent="0.4">
       <c r="A11" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C13" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F13" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="A12" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="10"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="A13" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="1:26" ht="30" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A14" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E14" s="10"/>
     </row>
-    <row r="15" spans="1:26" ht="53.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A15" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E15" s="10"/>
-      <c r="F15" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="16" spans="1:26" ht="30" x14ac:dyDescent="0.4">
       <c r="A16" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E16" s="10"/>
     </row>
-    <row r="17" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" ht="53.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="1:5" ht="39.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F17" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>59</v>
+      <c r="B18" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="E18" s="10"/>
     </row>
-    <row r="19" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>57</v>
+      <c r="B19" s="13" t="s">
+        <v>64</v>
       </c>
       <c r="E19" s="10"/>
     </row>
-    <row r="20" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" ht="39.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="10"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="E21" s="10"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="E23" s="10"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="E24" s="10"/>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="E25" s="10"/>
     </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="E26" s="10"/>
     </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E27" s="10"/>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E28" s="10"/>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E29" s="10"/>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E30" s="10"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E31" s="10"/>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E32" s="10"/>
     </row>
     <row r="33" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E33" s="10"/>
     </row>
-    <row r="34" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="35" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="34" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E34" s="10"/>
+    </row>
+    <row r="35" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E35" s="10"/>
+    </row>
     <row r="36" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="37" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="38" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1982,6 +2059,8 @@
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -1989,12 +2068,12 @@
     <hyperlink ref="F4" r:id="rId2" xr:uid="{B45A5CDE-8F77-412D-949B-8E8F551D8CC4}"/>
     <hyperlink ref="F5" r:id="rId3" xr:uid="{CA76DFB0-01D5-4DCB-9157-1E9F8E7412D9}"/>
     <hyperlink ref="F6" r:id="rId4" xr:uid="{83224FFE-86A0-488A-8F6A-FF6AF40ECC77}"/>
-    <hyperlink ref="F7" r:id="rId5" xr:uid="{45DF3FDE-3E99-4534-84FE-A28E806D5789}"/>
-    <hyperlink ref="F8" r:id="rId6" xr:uid="{084140FC-A1AF-405F-B226-87FB47D6A00E}"/>
-    <hyperlink ref="F9" r:id="rId7" xr:uid="{66F7160D-E8A6-449A-A5A8-658623D5755F}"/>
-    <hyperlink ref="F10" r:id="rId8" xr:uid="{90D560FD-8AB3-40D1-A390-4ABEF3D97AF8}"/>
-    <hyperlink ref="F11" r:id="rId9" display="https://web.dev/unused-css-rules/?utm_source=lighthouse&amp;utm_medium=devtools" xr:uid="{7B2C1893-7DB7-49FC-B823-A385BB686396}"/>
-    <hyperlink ref="F15" r:id="rId10" xr:uid="{AD3854B2-D1B6-442A-8257-485717595CD9}"/>
+    <hyperlink ref="F9" r:id="rId5" xr:uid="{45DF3FDE-3E99-4534-84FE-A28E806D5789}"/>
+    <hyperlink ref="F10" r:id="rId6" xr:uid="{084140FC-A1AF-405F-B226-87FB47D6A00E}"/>
+    <hyperlink ref="F11" r:id="rId7" xr:uid="{66F7160D-E8A6-449A-A5A8-658623D5755F}"/>
+    <hyperlink ref="F12" r:id="rId8" xr:uid="{90D560FD-8AB3-40D1-A390-4ABEF3D97AF8}"/>
+    <hyperlink ref="F13" r:id="rId9" display="https://web.dev/unused-css-rules/?utm_source=lighthouse&amp;utm_medium=devtools" xr:uid="{7B2C1893-7DB7-49FC-B823-A385BB686396}"/>
+    <hyperlink ref="F17" r:id="rId10" xr:uid="{AD3854B2-D1B6-442A-8257-485717595CD9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId11"/>

</xml_diff>

<commit_message>
add form label reduce style.css
</commit_message>
<xml_diff>
--- a/SEO-audit.xlsx
+++ b/SEO-audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OPENCLASSROOMS\PROJECT 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACD2225-061F-4491-9242-2CA758CE5D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB48967-63D3-4000-A7D2-23089202FA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="81">
   <si>
     <t>Category</t>
   </si>
@@ -321,6 +321,30 @@
   </si>
   <si>
     <t>https://web.dev/image-alt/?utm_source=lighthouse&amp;utm_medium=devtools</t>
+  </si>
+  <si>
+    <t>Form elements do not have associated labels (Page 2)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Labels ensure that form controls are announced properly by assistive technologies, like screen readers.</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://web.dev/label/?utm_source=lighthouse&amp;utm_medium=devtools</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Associate a label with a form element</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>use the label's for attribute and refer to the element's ID</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>import the correct css</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -689,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.27734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -873,191 +897,210 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="85.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:26" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="9" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="59.65" customHeight="1" x14ac:dyDescent="0.4">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="85.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="45" x14ac:dyDescent="0.4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="59.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="45" x14ac:dyDescent="0.4">
       <c r="A12" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C14" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D14" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F14" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="A14" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A15" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E15" s="10"/>
     </row>
-    <row r="16" spans="1:26" ht="30" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A16" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E16" s="10"/>
     </row>
-    <row r="17" spans="1:6" ht="53.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.4">
       <c r="A17" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E17" s="10"/>
-      <c r="F17" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="18" spans="1:6" ht="53.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F18" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E19" s="10"/>
     </row>
-    <row r="20" spans="1:6" ht="39.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E20" s="10"/>
-    </row>
-    <row r="21" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="39.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>57</v>
+      <c r="B21" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="E23" s="10"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.4">
@@ -1069,7 +1112,7 @@
     <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="E26" s="10"/>
     </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="E27" s="10"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1096,7 +1139,9 @@
     <row r="35" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E35" s="10"/>
     </row>
-    <row r="36" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="36" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E36" s="10"/>
+    </row>
     <row r="37" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="38" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="39" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -2061,6 +2106,7 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -2068,14 +2114,15 @@
     <hyperlink ref="F4" r:id="rId2" xr:uid="{B45A5CDE-8F77-412D-949B-8E8F551D8CC4}"/>
     <hyperlink ref="F5" r:id="rId3" xr:uid="{CA76DFB0-01D5-4DCB-9157-1E9F8E7412D9}"/>
     <hyperlink ref="F6" r:id="rId4" xr:uid="{83224FFE-86A0-488A-8F6A-FF6AF40ECC77}"/>
-    <hyperlink ref="F9" r:id="rId5" xr:uid="{45DF3FDE-3E99-4534-84FE-A28E806D5789}"/>
-    <hyperlink ref="F10" r:id="rId6" xr:uid="{084140FC-A1AF-405F-B226-87FB47D6A00E}"/>
-    <hyperlink ref="F11" r:id="rId7" xr:uid="{66F7160D-E8A6-449A-A5A8-658623D5755F}"/>
-    <hyperlink ref="F12" r:id="rId8" xr:uid="{90D560FD-8AB3-40D1-A390-4ABEF3D97AF8}"/>
-    <hyperlink ref="F13" r:id="rId9" display="https://web.dev/unused-css-rules/?utm_source=lighthouse&amp;utm_medium=devtools" xr:uid="{7B2C1893-7DB7-49FC-B823-A385BB686396}"/>
-    <hyperlink ref="F17" r:id="rId10" xr:uid="{AD3854B2-D1B6-442A-8257-485717595CD9}"/>
+    <hyperlink ref="F10" r:id="rId5" xr:uid="{45DF3FDE-3E99-4534-84FE-A28E806D5789}"/>
+    <hyperlink ref="F11" r:id="rId6" xr:uid="{084140FC-A1AF-405F-B226-87FB47D6A00E}"/>
+    <hyperlink ref="F12" r:id="rId7" xr:uid="{66F7160D-E8A6-449A-A5A8-658623D5755F}"/>
+    <hyperlink ref="F13" r:id="rId8" xr:uid="{90D560FD-8AB3-40D1-A390-4ABEF3D97AF8}"/>
+    <hyperlink ref="F14" r:id="rId9" display="https://web.dev/unused-css-rules/?utm_source=lighthouse&amp;utm_medium=devtools" xr:uid="{7B2C1893-7DB7-49FC-B823-A385BB686396}"/>
+    <hyperlink ref="F18" r:id="rId10" xr:uid="{AD3854B2-D1B6-442A-8257-485717595CD9}"/>
+    <hyperlink ref="F9" r:id="rId11" xr:uid="{3CDADFB8-264C-4418-BC68-A87AC6EA5E32}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId11"/>
+  <pageSetup orientation="landscape" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove alt spam words adjust social icon align type in mobile
</commit_message>
<xml_diff>
--- a/SEO-audit.xlsx
+++ b/SEO-audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OPENCLASSROOMS\PROJECT 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB48967-63D3-4000-A7D2-23089202FA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586BECE3-EA93-4150-BF95-E1B15D940E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
   <si>
     <t>Category</t>
   </si>
@@ -343,7 +343,15 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>import the correct css</t>
+    <t>Search engine users rely on the title to determine whether a page is relevant to their search.</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Make sure the title clearly states what the page is about. </t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Add a &lt;title&gt; element to the &lt;head&gt; of page. </t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -451,7 +459,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -490,6 +498,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -715,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.27734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1017,46 +1031,54 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" ht="53.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
+        <v>54</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E16" s="10"/>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" ht="36.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E17" s="10"/>
     </row>
-    <row r="18" spans="1:6" ht="53.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="51.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E18" s="10"/>
-      <c r="F18" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="19" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="9" t="s">
         <v>8</v>
       </c>
@@ -1065,69 +1087,67 @@
       </c>
       <c r="E19" s="10"/>
     </row>
-    <row r="20" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="39.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="1:5" ht="43.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="13" t="s">
         <v>59</v>
       </c>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="15" t="s">
         <v>57</v>
       </c>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="14" t="s">
         <v>58</v>
       </c>
       <c r="E23" s="10"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="E24" s="10"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="E25" s="10"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="E26" s="10"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="E27" s="10"/>
     </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E28" s="10"/>
     </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E29" s="10"/>
     </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E30" s="10"/>
     </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E31" s="10"/>
     </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E32" s="10"/>
     </row>
     <row r="33" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -2119,7 +2139,7 @@
     <hyperlink ref="F12" r:id="rId7" xr:uid="{66F7160D-E8A6-449A-A5A8-658623D5755F}"/>
     <hyperlink ref="F13" r:id="rId8" xr:uid="{90D560FD-8AB3-40D1-A390-4ABEF3D97AF8}"/>
     <hyperlink ref="F14" r:id="rId9" display="https://web.dev/unused-css-rules/?utm_source=lighthouse&amp;utm_medium=devtools" xr:uid="{7B2C1893-7DB7-49FC-B823-A385BB686396}"/>
-    <hyperlink ref="F18" r:id="rId10" xr:uid="{AD3854B2-D1B6-442A-8257-485717595CD9}"/>
+    <hyperlink ref="F15" r:id="rId10" xr:uid="{AD3854B2-D1B6-442A-8257-485717595CD9}"/>
     <hyperlink ref="F9" r:id="rId11" xr:uid="{3CDADFB8-264C-4418-BC68-A87AC6EA5E32}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>